<commit_message>
Base de datos nueva
Tablas de la base de datos que hicimos....
</commit_message>
<xml_diff>
--- a/Documentacion/tablas base de datos.xlsx
+++ b/Documentacion/tablas base de datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>id_dron</t>
   </si>
@@ -65,9 +65,6 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>Tipos</t>
-  </si>
-  <si>
     <t>Reporte Dron</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>cuadrante</t>
   </si>
   <si>
-    <t>diagnostico_id</t>
-  </si>
-  <si>
     <t>sintomas</t>
   </si>
   <si>
@@ -174,6 +168,36 @@
   </si>
   <si>
     <t xml:space="preserve">ap_materno </t>
+  </si>
+  <si>
+    <t>fecha_instalacion</t>
+  </si>
+  <si>
+    <t>imagen</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>Tipo_accidente</t>
+  </si>
+  <si>
+    <t>tipo_accidente_id</t>
+  </si>
+  <si>
+    <t>id_diagnostico</t>
+  </si>
+  <si>
+    <t>nombre_victima</t>
+  </si>
+  <si>
+    <t>ap_paterno_victima</t>
+  </si>
+  <si>
+    <t>ap_materno_victima</t>
+  </si>
+  <si>
+    <t>no_decesos</t>
   </si>
 </sst>
 </file>
@@ -356,13 +380,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -376,53 +400,6 @@
         <a:xfrm flipV="1">
           <a:off x="3762375" y="676275"/>
           <a:ext cx="1247775" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3752850" y="1257300"/>
-          <a:ext cx="2305050" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -592,15 +569,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>21167</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -609,8 +586,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4000500" y="676275"/>
-          <a:ext cx="1247775" cy="9525"/>
+          <a:off x="4434417" y="676276"/>
+          <a:ext cx="2323041" cy="11641"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -644,10 +621,10 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -656,8 +633,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3990975" y="1257300"/>
-          <a:ext cx="2305050" cy="762000"/>
+          <a:off x="4422775" y="1257300"/>
+          <a:ext cx="4266142" cy="1166283"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -848,8 +825,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E14:E23" totalsRowShown="0">
-  <autoFilter ref="E14:E23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E14:E25" totalsRowShown="0">
+  <autoFilter ref="E14:E25"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Reporte"/>
   </tableColumns>
@@ -861,15 +838,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="B12:B14" totalsRowShown="0">
   <autoFilter ref="B12:B14"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Tipos"/>
+    <tableColumn id="1" name="Tipo_accidente"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="F3:F7" totalsRowShown="0">
-  <autoFilter ref="F3:F7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="G3:G9" totalsRowShown="0">
+  <autoFilter ref="G3:G9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Drones"/>
   </tableColumns>
@@ -878,8 +855,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="G10:G15" totalsRowShown="0">
-  <autoFilter ref="G10:G15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="I12:I17" totalsRowShown="0">
+  <autoFilter ref="I12:I17"/>
   <tableColumns count="1">
     <tableColumn id="1" name="cuadrante"/>
   </tableColumns>
@@ -888,8 +865,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="G19:G26" totalsRowShown="0">
-  <autoFilter ref="G19:G26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="G19:G32" totalsRowShown="0">
+  <autoFilter ref="G19:G32"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Diagnostico"/>
   </tableColumns>
@@ -1170,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G31"/>
+  <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,242 +1159,275 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
       <c r="G22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
+      <c r="G27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>44</v>
+      <c r="G31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Requerimientos y bases de datos
EL excel pues yo no le movi a nada tal vez un diseñin o algo así
</commit_message>
<xml_diff>
--- a/Documentacion/tablas base de datos.xlsx
+++ b/Documentacion/tablas base de datos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Desktop\Project-Eagle\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estadias\Project-Eagle\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="F20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BD nueva y arduino :v:
Agregue cambios en la base de datos que dijimos y el random para arduino
</commit_message>
<xml_diff>
--- a/Documentacion/tablas base de datos.xlsx
+++ b/Documentacion/tablas base de datos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>id_dron</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>alta</t>
+  </si>
+  <si>
+    <t>fallecio</t>
   </si>
 </sst>
 </file>
@@ -290,53 +293,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Conector recto de flecha 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="2009776" y="2419350"/>
-          <a:ext cx="1752599" cy="1895475"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -430,63 +386,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19052</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Conector recto de flecha 17"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="4962526" y="2800350"/>
-          <a:ext cx="1085849" cy="1095375"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1058334</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -495,8 +404,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2009776" y="2419350"/>
-          <a:ext cx="1990724" cy="1895475"/>
+          <a:off x="2442635" y="2419351"/>
+          <a:ext cx="4246032" cy="4332816"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -666,15 +575,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1068917</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -683,8 +592,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="5200651" y="2800350"/>
-          <a:ext cx="1085849" cy="1095375"/>
+          <a:off x="5651500" y="2592917"/>
+          <a:ext cx="1047750" cy="4011084"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -828,8 +737,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E14:E25" totalsRowShown="0">
-  <autoFilter ref="E14:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="E13:E23" totalsRowShown="0">
+  <autoFilter ref="E13:E23"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Reporte"/>
   </tableColumns>
@@ -868,8 +777,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="G19:G32" totalsRowShown="0">
-  <autoFilter ref="G19:G32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="G22:G37" totalsRowShown="0">
+  <autoFilter ref="G22:G37"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Diagnostico"/>
   </tableColumns>
@@ -1150,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I32"/>
+  <dimension ref="B3:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,6 +1153,9 @@
       <c r="B13" t="s">
         <v>52</v>
       </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
       <c r="I13" t="s">
         <v>3</v>
       </c>
@@ -1253,7 +1165,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
@@ -1261,7 +1173,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
@@ -1269,7 +1181,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1280,7 +1192,7 @@
         <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I17" t="s">
         <v>20</v>
@@ -1291,7 +1203,7 @@
         <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1299,10 +1211,7 @@
         <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G19" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -1310,10 +1219,7 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -1321,10 +1227,7 @@
         <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -1332,10 +1235,10 @@
         <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -1343,32 +1246,26 @@
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E24" t="s">
-        <v>57</v>
-      </c>
       <c r="G24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>23</v>
-      </c>
-      <c r="G25" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1376,7 +1273,7 @@
         <v>37</v>
       </c>
       <c r="G26" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -1384,7 +1281,7 @@
         <v>38</v>
       </c>
       <c r="G27" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -1395,7 +1292,7 @@
         <v>43</v>
       </c>
       <c r="G28" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -1406,7 +1303,7 @@
         <v>42</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -1417,7 +1314,7 @@
         <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -1425,7 +1322,7 @@
         <v>42</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -1433,7 +1330,32 @@
         <v>58</v>
       </c>
       <c r="G32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>